<commit_message>
Add device online status poll function. BedivereKnx and it's GUI will rename to BedwyrKnx and stop updating, BedivereKnx_CS will replace it.
</commit_message>
<xml_diff>
--- a/BedivereKnx_CS.test/data.xlsx
+++ b/BedivereKnx_CS.test/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Program\Ouroboros\BedivereKnx\BedivereKnx_CS.test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D10588C-82BD-4691-B814-7FEC1AF4E7AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616FA4C1-F26E-45A4-9BF2-B2698CD588E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Interfaces" sheetId="4" r:id="rId1"/>
@@ -206,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3859" uniqueCount="2127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3899" uniqueCount="2143">
   <si>
     <t>AreaCode</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -6724,6 +6724,70 @@
   </si>
   <si>
     <t>IpTunneling</t>
+  </si>
+  <si>
+    <t>TestA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TA1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TestA1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TA11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TestA11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TA12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TestA12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TA2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TestA2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TA21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TA22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TestA21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TestA22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TA23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TestA23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -7320,11 +7384,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -7423,7 +7487,7 @@
         <v>458</v>
       </c>
       <c r="G5" t="str">
-        <f t="shared" ref="G5:G28" si="0">A5&amp;IF(C5="","","."&amp;C5)&amp;IF(E5="","","."&amp;E5)</f>
+        <f t="shared" ref="G5:G38" si="0">A5&amp;IF(C5="","","."&amp;C5)&amp;IF(E5="","","."&amp;E5)</f>
         <v>Bld01.B01</v>
       </c>
     </row>
@@ -7821,6 +7885,174 @@
       <c r="G28" t="str">
         <f t="shared" si="0"/>
         <v>Garage</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>2128</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>2127</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="0"/>
+        <v>TA</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>2128</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>2127</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>2129</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>2130</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="0"/>
+        <v>TA.TA1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>2128</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>2127</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>2129</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>2130</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>2131</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>2132</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="0"/>
+        <v>TA.TA1.TA11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>2128</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>2127</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>2129</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>2130</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>2133</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>2134</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="0"/>
+        <v>TA.TA1.TA12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>2128</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>2127</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>2135</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>2136</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="0"/>
+        <v>TA.TA2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>2128</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>2127</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>2135</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>2136</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>2137</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>2139</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="0"/>
+        <v>TA.TA2.TA21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>2128</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>2127</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>2135</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>2136</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>2138</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>2140</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="0"/>
+        <v>TA.TA2.TA22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>2128</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>2127</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>2135</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>2136</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>2141</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>2142</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" ref="G36" si="2">A36&amp;IF(C36="","","."&amp;C36)&amp;IF(E36="","","."&amp;E36)</f>
+        <v>TA.TA2.TA23</v>
       </c>
     </row>
   </sheetData>
@@ -7834,7 +8066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE9671D8-C670-4FF9-9F5F-C699E4CE0AC7}">
   <dimension ref="A1:K446"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>

</xml_diff>